<commit_message>
Worked on Screenshot and Retry listener
</commit_message>
<xml_diff>
--- a/automationtraining/testdata.xlsx
+++ b/automationtraining/testdata.xlsx
@@ -3,29 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSTEMP194\git\automationtraining\automationtraining\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A08D841-DE45-4D3E-BC62-6DD696B55577}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6F8C0EAD-4DF2-45B3-B91A-7F6B39836851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="2160" xr2:uid="{221D4FD3-E661-4E3B-8080-3B00F72440CB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5835" xr2:uid="{221D4FD3-E661-4E3B-8080-3B00F72440CB}"/>
   </bookViews>
   <sheets>
     <sheet name="formFilling101" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -211,7 +200,7 @@
     <t>TCAT_101</t>
   </si>
   <si>
-    <t>sindhuja.e@mstsolutions.com</t>
+    <t>sindhube19.data@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -578,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44D3B42-8979-4DAD-92A6-CDE1B767810B}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +599,7 @@
     <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -841,7 +830,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AK2" r:id="rId1" xr:uid="{E0F8A47A-0690-470C-BC5E-1021788E37E7}"/>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{3B7DADEE-F490-4EC2-9383-9EF973B7FCFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on form data verification
</commit_message>
<xml_diff>
--- a/automationtraining/testdata.xlsx
+++ b/automationtraining/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2DAFEF89-555A-4743-99C4-4CD485233507}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FDDB4BA8-DED6-4AC1-A144-08DEB76EC162}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5835" xr2:uid="{221D4FD3-E661-4E3B-8080-3B00F72440CB}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <t>TCAT_101</t>
   </si>
   <si>
-    <t>sindhube19</t>
+    <t>sindhube19.data@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AK2" r:id="rId1" display="sindhube19.data@gmail.com" xr:uid="{3B7DADEE-F490-4EC2-9383-9EF973B7FCFF}"/>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{3B7DADEE-F490-4EC2-9383-9EF973B7FCFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>